<commit_message>
set correct name of indicator
</commit_message>
<xml_diff>
--- a/make_final_data/data/legend.xlsx
+++ b/make_final_data/data/legend.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucac\Desktop\make_final_data\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca_efti/Desktop/oltp_to_olap/make_final_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE484D61-2DC8-4C52-83A4-2C89EF9EF960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B803438-326B-9B47-8F73-7EF7921096E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -665,18 +665,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="151.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="151.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
@@ -687,7 +687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>53</v>
       </c>
@@ -698,7 +698,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -709,7 +709,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -720,7 +720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -731,7 +731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -742,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -753,7 +753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -764,7 +764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -775,7 +775,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -786,7 +786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -797,7 +797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -808,7 +808,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -819,7 +819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -848,14 +848,14 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -866,7 +866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
@@ -883,7 +883,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
@@ -900,7 +900,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
@@ -917,7 +917,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -928,7 +928,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -939,7 +939,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -950,7 +950,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -961,7 +961,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
@@ -972,7 +972,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -989,7 +989,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>58</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1069,14 +1069,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>44</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>62</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>57</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>55</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>56</v>
       </c>

</xml_diff>